<commit_message>
Fix transfer deficit report filters and aggregation
</commit_message>
<xml_diff>
--- a/plan of sales.xlsx
+++ b/plan of sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\668\so-planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBEC6B3-AFA9-4018-BE75-1D6D49400736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4372D1C0-2A3E-4FD3-B4C2-D7E27BC8DBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="2805" windowWidth="38700" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="5220" windowWidth="38700" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -363,8 +363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:MG12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BZ7" sqref="BZ7"/>
+    <sheetView tabSelected="1" topLeftCell="CW1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="DP3" sqref="DP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,16 +1414,25 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="BZ2">
-        <v>5500000</v>
+      <c r="DA2">
+        <v>10000</v>
+      </c>
+      <c r="DF2">
+        <v>10000</v>
+      </c>
+      <c r="DI2">
+        <v>10000</v>
+      </c>
+      <c r="DM2">
+        <v>10000</v>
+      </c>
+      <c r="DP2">
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>400000011</v>
-      </c>
-      <c r="CA3">
-        <v>8000</v>
       </c>
     </row>
     <row r="4" spans="1:345" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add updated BOM, plan data, and UI/API changes
</commit_message>
<xml_diff>
--- a/plan of sales.xlsx
+++ b/plan of sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\668\so-planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4372D1C0-2A3E-4FD3-B4C2-D7E27BC8DBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C38C25-8639-45D1-B48E-B474B83ADF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="5220" windowWidth="38700" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6465" yWindow="5760" windowWidth="38670" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -364,7 +364,7 @@
   <dimension ref="A1:MG12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CW1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="DP3" sqref="DP3"/>
+      <selection activeCell="DO2" sqref="DO2:DU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,19 +1414,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="DA2">
-        <v>10000</v>
-      </c>
-      <c r="DF2">
-        <v>10000</v>
-      </c>
-      <c r="DI2">
-        <v>10000</v>
-      </c>
-      <c r="DM2">
-        <v>10000</v>
-      </c>
-      <c r="DP2">
+      <c r="DN2">
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sync local planner updates and refresh docs/dependencies
</commit_message>
<xml_diff>
--- a/plan of sales.xlsx
+++ b/plan of sales.xlsx
@@ -5,29 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\668\so-planner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\so planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C38C25-8639-45D1-B48E-B474B83ADF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159DA231-B524-49A9-BDF2-300B9A385174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="5760" windowWidth="38670" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -361,1111 +352,867 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:MG12"/>
+  <dimension ref="A1:IW13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CW1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="DO2" sqref="DO2:DU2"/>
+    <sheetView tabSelected="1" topLeftCell="CF1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="CS11" sqref="CS11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" style="2" customWidth="1"/>
-    <col min="2" max="345" width="11" customWidth="1"/>
+    <col min="2" max="257" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>45983</v>
+        <v>46071</v>
       </c>
       <c r="C1" s="1">
-        <v>45984</v>
+        <v>46072</v>
       </c>
       <c r="D1" s="1">
-        <v>45985</v>
+        <v>46073</v>
       </c>
       <c r="E1" s="1">
-        <v>45986</v>
+        <v>46074</v>
       </c>
       <c r="F1" s="1">
-        <v>45987</v>
+        <v>46075</v>
       </c>
       <c r="G1" s="1">
-        <v>45988</v>
+        <v>46076</v>
       </c>
       <c r="H1" s="1">
-        <v>45989</v>
+        <v>46077</v>
       </c>
       <c r="I1" s="1">
-        <v>45990</v>
+        <v>46078</v>
       </c>
       <c r="J1" s="1">
-        <v>45991</v>
+        <v>46079</v>
       </c>
       <c r="K1" s="1">
-        <v>45992</v>
+        <v>46080</v>
       </c>
       <c r="L1" s="1">
-        <v>45993</v>
+        <v>46081</v>
       </c>
       <c r="M1" s="1">
-        <v>45994</v>
+        <v>46082</v>
       </c>
       <c r="N1" s="1">
-        <v>45995</v>
+        <v>46083</v>
       </c>
       <c r="O1" s="1">
-        <v>45996</v>
+        <v>46084</v>
       </c>
       <c r="P1" s="1">
-        <v>45997</v>
+        <v>46085</v>
       </c>
       <c r="Q1" s="1">
-        <v>45998</v>
+        <v>46086</v>
       </c>
       <c r="R1" s="1">
-        <v>45999</v>
+        <v>46087</v>
       </c>
       <c r="S1" s="1">
-        <v>46000</v>
+        <v>46088</v>
       </c>
       <c r="T1" s="1">
-        <v>46001</v>
+        <v>46089</v>
       </c>
       <c r="U1" s="1">
-        <v>46002</v>
+        <v>46090</v>
       </c>
       <c r="V1" s="1">
-        <v>46003</v>
+        <v>46091</v>
       </c>
       <c r="W1" s="1">
-        <v>46004</v>
+        <v>46092</v>
       </c>
       <c r="X1" s="1">
-        <v>46005</v>
+        <v>46093</v>
       </c>
       <c r="Y1" s="1">
-        <v>46006</v>
+        <v>46094</v>
       </c>
       <c r="Z1" s="1">
-        <v>46007</v>
+        <v>46095</v>
       </c>
       <c r="AA1" s="1">
-        <v>46008</v>
+        <v>46096</v>
       </c>
       <c r="AB1" s="1">
-        <v>46009</v>
+        <v>46097</v>
       </c>
       <c r="AC1" s="1">
-        <v>46010</v>
+        <v>46098</v>
       </c>
       <c r="AD1" s="1">
-        <v>46011</v>
+        <v>46099</v>
       </c>
       <c r="AE1" s="1">
-        <v>46012</v>
+        <v>46100</v>
       </c>
       <c r="AF1" s="1">
-        <v>46013</v>
+        <v>46101</v>
       </c>
       <c r="AG1" s="1">
-        <v>46014</v>
+        <v>46102</v>
       </c>
       <c r="AH1" s="1">
-        <v>46015</v>
+        <v>46103</v>
       </c>
       <c r="AI1" s="1">
-        <v>46016</v>
+        <v>46104</v>
       </c>
       <c r="AJ1" s="1">
-        <v>46017</v>
+        <v>46105</v>
       </c>
       <c r="AK1" s="1">
-        <v>46018</v>
+        <v>46106</v>
       </c>
       <c r="AL1" s="1">
-        <v>46019</v>
+        <v>46107</v>
       </c>
       <c r="AM1" s="1">
-        <v>46020</v>
+        <v>46108</v>
       </c>
       <c r="AN1" s="1">
-        <v>46021</v>
+        <v>46109</v>
       </c>
       <c r="AO1" s="1">
-        <v>46022</v>
+        <v>46110</v>
       </c>
       <c r="AP1" s="1">
-        <v>46023</v>
+        <v>46111</v>
       </c>
       <c r="AQ1" s="1">
-        <v>46024</v>
+        <v>46112</v>
       </c>
       <c r="AR1" s="1">
-        <v>46025</v>
+        <v>46113</v>
       </c>
       <c r="AS1" s="1">
-        <v>46026</v>
+        <v>46114</v>
       </c>
       <c r="AT1" s="1">
-        <v>46027</v>
+        <v>46115</v>
       </c>
       <c r="AU1" s="1">
-        <v>46028</v>
+        <v>46116</v>
       </c>
       <c r="AV1" s="1">
-        <v>46029</v>
+        <v>46117</v>
       </c>
       <c r="AW1" s="1">
-        <v>46030</v>
+        <v>46118</v>
       </c>
       <c r="AX1" s="1">
-        <v>46031</v>
+        <v>46119</v>
       </c>
       <c r="AY1" s="1">
-        <v>46032</v>
+        <v>46120</v>
       </c>
       <c r="AZ1" s="1">
-        <v>46033</v>
+        <v>46121</v>
       </c>
       <c r="BA1" s="1">
-        <v>46034</v>
+        <v>46122</v>
       </c>
       <c r="BB1" s="1">
-        <v>46035</v>
+        <v>46123</v>
       </c>
       <c r="BC1" s="1">
-        <v>46036</v>
+        <v>46124</v>
       </c>
       <c r="BD1" s="1">
-        <v>46037</v>
+        <v>46125</v>
       </c>
       <c r="BE1" s="1">
-        <v>46038</v>
+        <v>46126</v>
       </c>
       <c r="BF1" s="1">
-        <v>46039</v>
+        <v>46127</v>
       </c>
       <c r="BG1" s="1">
-        <v>46040</v>
+        <v>46128</v>
       </c>
       <c r="BH1" s="1">
-        <v>46041</v>
+        <v>46129</v>
       </c>
       <c r="BI1" s="1">
-        <v>46042</v>
+        <v>46130</v>
       </c>
       <c r="BJ1" s="1">
-        <v>46043</v>
+        <v>46131</v>
       </c>
       <c r="BK1" s="1">
-        <v>46044</v>
+        <v>46132</v>
       </c>
       <c r="BL1" s="1">
-        <v>46045</v>
+        <v>46133</v>
       </c>
       <c r="BM1" s="1">
-        <v>46046</v>
+        <v>46134</v>
       </c>
       <c r="BN1" s="1">
-        <v>46047</v>
+        <v>46135</v>
       </c>
       <c r="BO1" s="1">
-        <v>46048</v>
+        <v>46136</v>
       </c>
       <c r="BP1" s="1">
-        <v>46049</v>
+        <v>46137</v>
       </c>
       <c r="BQ1" s="1">
-        <v>46050</v>
+        <v>46138</v>
       </c>
       <c r="BR1" s="1">
-        <v>46051</v>
+        <v>46139</v>
       </c>
       <c r="BS1" s="1">
-        <v>46052</v>
+        <v>46140</v>
       </c>
       <c r="BT1" s="1">
-        <v>46053</v>
+        <v>46141</v>
       </c>
       <c r="BU1" s="1">
-        <v>46054</v>
+        <v>46142</v>
       </c>
       <c r="BV1" s="1">
-        <v>46055</v>
+        <v>46143</v>
       </c>
       <c r="BW1" s="1">
-        <v>46056</v>
+        <v>46144</v>
       </c>
       <c r="BX1" s="1">
-        <v>46057</v>
+        <v>46145</v>
       </c>
       <c r="BY1" s="1">
-        <v>46058</v>
+        <v>46146</v>
       </c>
       <c r="BZ1" s="1">
-        <v>46059</v>
+        <v>46147</v>
       </c>
       <c r="CA1" s="1">
-        <v>46060</v>
+        <v>46148</v>
       </c>
       <c r="CB1" s="1">
-        <v>46061</v>
+        <v>46149</v>
       </c>
       <c r="CC1" s="1">
-        <v>46062</v>
+        <v>46150</v>
       </c>
       <c r="CD1" s="1">
-        <v>46063</v>
+        <v>46151</v>
       </c>
       <c r="CE1" s="1">
-        <v>46064</v>
+        <v>46152</v>
       </c>
       <c r="CF1" s="1">
-        <v>46065</v>
+        <v>46153</v>
       </c>
       <c r="CG1" s="1">
-        <v>46066</v>
+        <v>46154</v>
       </c>
       <c r="CH1" s="1">
-        <v>46067</v>
+        <v>46155</v>
       </c>
       <c r="CI1" s="1">
-        <v>46068</v>
+        <v>46156</v>
       </c>
       <c r="CJ1" s="1">
-        <v>46069</v>
+        <v>46157</v>
       </c>
       <c r="CK1" s="1">
-        <v>46070</v>
+        <v>46158</v>
       </c>
       <c r="CL1" s="1">
-        <v>46071</v>
+        <v>46159</v>
       </c>
       <c r="CM1" s="1">
-        <v>46072</v>
+        <v>46160</v>
       </c>
       <c r="CN1" s="1">
-        <v>46073</v>
+        <v>46161</v>
       </c>
       <c r="CO1" s="1">
-        <v>46074</v>
+        <v>46162</v>
       </c>
       <c r="CP1" s="1">
-        <v>46075</v>
+        <v>46163</v>
       </c>
       <c r="CQ1" s="1">
-        <v>46076</v>
+        <v>46164</v>
       </c>
       <c r="CR1" s="1">
-        <v>46077</v>
+        <v>46165</v>
       </c>
       <c r="CS1" s="1">
-        <v>46078</v>
+        <v>46166</v>
       </c>
       <c r="CT1" s="1">
-        <v>46079</v>
+        <v>46167</v>
       </c>
       <c r="CU1" s="1">
-        <v>46080</v>
+        <v>46168</v>
       </c>
       <c r="CV1" s="1">
-        <v>46081</v>
+        <v>46169</v>
       </c>
       <c r="CW1" s="1">
-        <v>46082</v>
+        <v>46170</v>
       </c>
       <c r="CX1" s="1">
-        <v>46083</v>
+        <v>46171</v>
       </c>
       <c r="CY1" s="1">
-        <v>46084</v>
+        <v>46172</v>
       </c>
       <c r="CZ1" s="1">
-        <v>46085</v>
+        <v>46173</v>
       </c>
       <c r="DA1" s="1">
-        <v>46086</v>
+        <v>46174</v>
       </c>
       <c r="DB1" s="1">
-        <v>46087</v>
+        <v>46175</v>
       </c>
       <c r="DC1" s="1">
-        <v>46088</v>
+        <v>46176</v>
       </c>
       <c r="DD1" s="1">
-        <v>46089</v>
+        <v>46177</v>
       </c>
       <c r="DE1" s="1">
-        <v>46090</v>
+        <v>46178</v>
       </c>
       <c r="DF1" s="1">
-        <v>46091</v>
+        <v>46179</v>
       </c>
       <c r="DG1" s="1">
-        <v>46092</v>
+        <v>46180</v>
       </c>
       <c r="DH1" s="1">
-        <v>46093</v>
+        <v>46181</v>
       </c>
       <c r="DI1" s="1">
-        <v>46094</v>
+        <v>46182</v>
       </c>
       <c r="DJ1" s="1">
-        <v>46095</v>
+        <v>46183</v>
       </c>
       <c r="DK1" s="1">
-        <v>46096</v>
+        <v>46184</v>
       </c>
       <c r="DL1" s="1">
-        <v>46097</v>
+        <v>46185</v>
       </c>
       <c r="DM1" s="1">
-        <v>46098</v>
+        <v>46186</v>
       </c>
       <c r="DN1" s="1">
-        <v>46099</v>
+        <v>46187</v>
       </c>
       <c r="DO1" s="1">
-        <v>46100</v>
+        <v>46188</v>
       </c>
       <c r="DP1" s="1">
-        <v>46101</v>
+        <v>46189</v>
       </c>
       <c r="DQ1" s="1">
-        <v>46102</v>
+        <v>46190</v>
       </c>
       <c r="DR1" s="1">
-        <v>46103</v>
+        <v>46191</v>
       </c>
       <c r="DS1" s="1">
-        <v>46104</v>
+        <v>46192</v>
       </c>
       <c r="DT1" s="1">
-        <v>46105</v>
+        <v>46193</v>
       </c>
       <c r="DU1" s="1">
-        <v>46106</v>
+        <v>46194</v>
       </c>
       <c r="DV1" s="1">
-        <v>46107</v>
+        <v>46195</v>
       </c>
       <c r="DW1" s="1">
-        <v>46108</v>
+        <v>46196</v>
       </c>
       <c r="DX1" s="1">
-        <v>46109</v>
+        <v>46197</v>
       </c>
       <c r="DY1" s="1">
-        <v>46110</v>
+        <v>46198</v>
       </c>
       <c r="DZ1" s="1">
-        <v>46111</v>
+        <v>46199</v>
       </c>
       <c r="EA1" s="1">
-        <v>46112</v>
+        <v>46200</v>
       </c>
       <c r="EB1" s="1">
-        <v>46113</v>
+        <v>46201</v>
       </c>
       <c r="EC1" s="1">
-        <v>46114</v>
+        <v>46202</v>
       </c>
       <c r="ED1" s="1">
-        <v>46115</v>
+        <v>46203</v>
       </c>
       <c r="EE1" s="1">
-        <v>46116</v>
+        <v>46204</v>
       </c>
       <c r="EF1" s="1">
-        <v>46117</v>
+        <v>46205</v>
       </c>
       <c r="EG1" s="1">
-        <v>46118</v>
+        <v>46206</v>
       </c>
       <c r="EH1" s="1">
-        <v>46119</v>
+        <v>46207</v>
       </c>
       <c r="EI1" s="1">
-        <v>46120</v>
+        <v>46208</v>
       </c>
       <c r="EJ1" s="1">
-        <v>46121</v>
+        <v>46209</v>
       </c>
       <c r="EK1" s="1">
-        <v>46122</v>
+        <v>46210</v>
       </c>
       <c r="EL1" s="1">
-        <v>46123</v>
+        <v>46211</v>
       </c>
       <c r="EM1" s="1">
-        <v>46124</v>
+        <v>46212</v>
       </c>
       <c r="EN1" s="1">
-        <v>46125</v>
+        <v>46213</v>
       </c>
       <c r="EO1" s="1">
-        <v>46126</v>
+        <v>46214</v>
       </c>
       <c r="EP1" s="1">
-        <v>46127</v>
+        <v>46215</v>
       </c>
       <c r="EQ1" s="1">
-        <v>46128</v>
+        <v>46216</v>
       </c>
       <c r="ER1" s="1">
-        <v>46129</v>
+        <v>46217</v>
       </c>
       <c r="ES1" s="1">
-        <v>46130</v>
+        <v>46218</v>
       </c>
       <c r="ET1" s="1">
-        <v>46131</v>
+        <v>46219</v>
       </c>
       <c r="EU1" s="1">
-        <v>46132</v>
+        <v>46220</v>
       </c>
       <c r="EV1" s="1">
-        <v>46133</v>
+        <v>46221</v>
       </c>
       <c r="EW1" s="1">
-        <v>46134</v>
+        <v>46222</v>
       </c>
       <c r="EX1" s="1">
-        <v>46135</v>
+        <v>46223</v>
       </c>
       <c r="EY1" s="1">
-        <v>46136</v>
+        <v>46224</v>
       </c>
       <c r="EZ1" s="1">
-        <v>46137</v>
+        <v>46225</v>
       </c>
       <c r="FA1" s="1">
-        <v>46138</v>
+        <v>46226</v>
       </c>
       <c r="FB1" s="1">
-        <v>46139</v>
+        <v>46227</v>
       </c>
       <c r="FC1" s="1">
-        <v>46140</v>
+        <v>46228</v>
       </c>
       <c r="FD1" s="1">
-        <v>46141</v>
+        <v>46229</v>
       </c>
       <c r="FE1" s="1">
-        <v>46142</v>
+        <v>46230</v>
       </c>
       <c r="FF1" s="1">
-        <v>46143</v>
+        <v>46231</v>
       </c>
       <c r="FG1" s="1">
-        <v>46144</v>
+        <v>46232</v>
       </c>
       <c r="FH1" s="1">
-        <v>46145</v>
+        <v>46233</v>
       </c>
       <c r="FI1" s="1">
-        <v>46146</v>
+        <v>46234</v>
       </c>
       <c r="FJ1" s="1">
-        <v>46147</v>
+        <v>46235</v>
       </c>
       <c r="FK1" s="1">
-        <v>46148</v>
+        <v>46236</v>
       </c>
       <c r="FL1" s="1">
-        <v>46149</v>
+        <v>46237</v>
       </c>
       <c r="FM1" s="1">
-        <v>46150</v>
+        <v>46238</v>
       </c>
       <c r="FN1" s="1">
-        <v>46151</v>
+        <v>46239</v>
       </c>
       <c r="FO1" s="1">
-        <v>46152</v>
+        <v>46240</v>
       </c>
       <c r="FP1" s="1">
-        <v>46153</v>
+        <v>46241</v>
       </c>
       <c r="FQ1" s="1">
-        <v>46154</v>
+        <v>46242</v>
       </c>
       <c r="FR1" s="1">
-        <v>46155</v>
+        <v>46243</v>
       </c>
       <c r="FS1" s="1">
-        <v>46156</v>
+        <v>46244</v>
       </c>
       <c r="FT1" s="1">
-        <v>46157</v>
+        <v>46245</v>
       </c>
       <c r="FU1" s="1">
-        <v>46158</v>
+        <v>46246</v>
       </c>
       <c r="FV1" s="1">
-        <v>46159</v>
+        <v>46247</v>
       </c>
       <c r="FW1" s="1">
-        <v>46160</v>
+        <v>46248</v>
       </c>
       <c r="FX1" s="1">
-        <v>46161</v>
+        <v>46249</v>
       </c>
       <c r="FY1" s="1">
-        <v>46162</v>
+        <v>46250</v>
       </c>
       <c r="FZ1" s="1">
-        <v>46163</v>
+        <v>46251</v>
       </c>
       <c r="GA1" s="1">
-        <v>46164</v>
+        <v>46252</v>
       </c>
       <c r="GB1" s="1">
-        <v>46165</v>
+        <v>46253</v>
       </c>
       <c r="GC1" s="1">
-        <v>46166</v>
+        <v>46254</v>
       </c>
       <c r="GD1" s="1">
-        <v>46167</v>
+        <v>46255</v>
       </c>
       <c r="GE1" s="1">
-        <v>46168</v>
+        <v>46256</v>
       </c>
       <c r="GF1" s="1">
-        <v>46169</v>
+        <v>46257</v>
       </c>
       <c r="GG1" s="1">
-        <v>46170</v>
+        <v>46258</v>
       </c>
       <c r="GH1" s="1">
-        <v>46171</v>
+        <v>46259</v>
       </c>
       <c r="GI1" s="1">
-        <v>46172</v>
+        <v>46260</v>
       </c>
       <c r="GJ1" s="1">
-        <v>46173</v>
+        <v>46261</v>
       </c>
       <c r="GK1" s="1">
-        <v>46174</v>
+        <v>46262</v>
       </c>
       <c r="GL1" s="1">
-        <v>46175</v>
+        <v>46263</v>
       </c>
       <c r="GM1" s="1">
-        <v>46176</v>
+        <v>46264</v>
       </c>
       <c r="GN1" s="1">
-        <v>46177</v>
+        <v>46265</v>
       </c>
       <c r="GO1" s="1">
-        <v>46178</v>
+        <v>46266</v>
       </c>
       <c r="GP1" s="1">
-        <v>46179</v>
+        <v>46267</v>
       </c>
       <c r="GQ1" s="1">
-        <v>46180</v>
+        <v>46268</v>
       </c>
       <c r="GR1" s="1">
-        <v>46181</v>
+        <v>46269</v>
       </c>
       <c r="GS1" s="1">
-        <v>46182</v>
+        <v>46270</v>
       </c>
       <c r="GT1" s="1">
-        <v>46183</v>
+        <v>46271</v>
       </c>
       <c r="GU1" s="1">
-        <v>46184</v>
+        <v>46272</v>
       </c>
       <c r="GV1" s="1">
-        <v>46185</v>
+        <v>46273</v>
       </c>
       <c r="GW1" s="1">
-        <v>46186</v>
+        <v>46274</v>
       </c>
       <c r="GX1" s="1">
-        <v>46187</v>
+        <v>46275</v>
       </c>
       <c r="GY1" s="1">
-        <v>46188</v>
+        <v>46276</v>
       </c>
       <c r="GZ1" s="1">
-        <v>46189</v>
+        <v>46277</v>
       </c>
       <c r="HA1" s="1">
-        <v>46190</v>
+        <v>46278</v>
       </c>
       <c r="HB1" s="1">
-        <v>46191</v>
+        <v>46279</v>
       </c>
       <c r="HC1" s="1">
-        <v>46192</v>
+        <v>46280</v>
       </c>
       <c r="HD1" s="1">
-        <v>46193</v>
+        <v>46281</v>
       </c>
       <c r="HE1" s="1">
-        <v>46194</v>
+        <v>46282</v>
       </c>
       <c r="HF1" s="1">
-        <v>46195</v>
+        <v>46283</v>
       </c>
       <c r="HG1" s="1">
-        <v>46196</v>
+        <v>46284</v>
       </c>
       <c r="HH1" s="1">
-        <v>46197</v>
+        <v>46285</v>
       </c>
       <c r="HI1" s="1">
-        <v>46198</v>
+        <v>46286</v>
       </c>
       <c r="HJ1" s="1">
-        <v>46199</v>
+        <v>46287</v>
       </c>
       <c r="HK1" s="1">
-        <v>46200</v>
+        <v>46288</v>
       </c>
       <c r="HL1" s="1">
-        <v>46201</v>
+        <v>46289</v>
       </c>
       <c r="HM1" s="1">
-        <v>46202</v>
+        <v>46290</v>
       </c>
       <c r="HN1" s="1">
-        <v>46203</v>
+        <v>46291</v>
       </c>
       <c r="HO1" s="1">
-        <v>46204</v>
+        <v>46292</v>
       </c>
       <c r="HP1" s="1">
-        <v>46205</v>
+        <v>46293</v>
       </c>
       <c r="HQ1" s="1">
-        <v>46206</v>
+        <v>46294</v>
       </c>
       <c r="HR1" s="1">
-        <v>46207</v>
+        <v>46295</v>
       </c>
       <c r="HS1" s="1">
-        <v>46208</v>
+        <v>46296</v>
       </c>
       <c r="HT1" s="1">
-        <v>46209</v>
+        <v>46297</v>
       </c>
       <c r="HU1" s="1">
-        <v>46210</v>
+        <v>46298</v>
       </c>
       <c r="HV1" s="1">
-        <v>46211</v>
+        <v>46299</v>
       </c>
       <c r="HW1" s="1">
-        <v>46212</v>
+        <v>46300</v>
       </c>
       <c r="HX1" s="1">
-        <v>46213</v>
+        <v>46301</v>
       </c>
       <c r="HY1" s="1">
-        <v>46214</v>
+        <v>46302</v>
       </c>
       <c r="HZ1" s="1">
-        <v>46215</v>
+        <v>46303</v>
       </c>
       <c r="IA1" s="1">
-        <v>46216</v>
+        <v>46304</v>
       </c>
       <c r="IB1" s="1">
-        <v>46217</v>
+        <v>46305</v>
       </c>
       <c r="IC1" s="1">
-        <v>46218</v>
+        <v>46306</v>
       </c>
       <c r="ID1" s="1">
-        <v>46219</v>
+        <v>46307</v>
       </c>
       <c r="IE1" s="1">
-        <v>46220</v>
+        <v>46308</v>
       </c>
       <c r="IF1" s="1">
-        <v>46221</v>
+        <v>46309</v>
       </c>
       <c r="IG1" s="1">
-        <v>46222</v>
+        <v>46310</v>
       </c>
       <c r="IH1" s="1">
-        <v>46223</v>
+        <v>46311</v>
       </c>
       <c r="II1" s="1">
-        <v>46224</v>
+        <v>46312</v>
       </c>
       <c r="IJ1" s="1">
-        <v>46225</v>
+        <v>46313</v>
       </c>
       <c r="IK1" s="1">
-        <v>46226</v>
+        <v>46314</v>
       </c>
       <c r="IL1" s="1">
-        <v>46227</v>
+        <v>46315</v>
       </c>
       <c r="IM1" s="1">
-        <v>46228</v>
+        <v>46316</v>
       </c>
       <c r="IN1" s="1">
-        <v>46229</v>
+        <v>46317</v>
       </c>
       <c r="IO1" s="1">
-        <v>46230</v>
+        <v>46318</v>
       </c>
       <c r="IP1" s="1">
-        <v>46231</v>
+        <v>46319</v>
       </c>
       <c r="IQ1" s="1">
-        <v>46232</v>
+        <v>46320</v>
       </c>
       <c r="IR1" s="1">
-        <v>46233</v>
+        <v>46321</v>
       </c>
       <c r="IS1" s="1">
-        <v>46234</v>
+        <v>46322</v>
       </c>
       <c r="IT1" s="1">
-        <v>46235</v>
+        <v>46323</v>
       </c>
       <c r="IU1" s="1">
-        <v>46236</v>
+        <v>46324</v>
       </c>
       <c r="IV1" s="1">
-        <v>46237</v>
+        <v>46325</v>
       </c>
       <c r="IW1" s="1">
-        <v>46238</v>
-      </c>
-      <c r="IX1" s="1">
-        <v>46239</v>
-      </c>
-      <c r="IY1" s="1">
-        <v>46240</v>
-      </c>
-      <c r="IZ1" s="1">
-        <v>46241</v>
-      </c>
-      <c r="JA1" s="1">
-        <v>46242</v>
-      </c>
-      <c r="JB1" s="1">
-        <v>46243</v>
-      </c>
-      <c r="JC1" s="1">
-        <v>46244</v>
-      </c>
-      <c r="JD1" s="1">
-        <v>46245</v>
-      </c>
-      <c r="JE1" s="1">
-        <v>46246</v>
-      </c>
-      <c r="JF1" s="1">
-        <v>46247</v>
-      </c>
-      <c r="JG1" s="1">
-        <v>46248</v>
-      </c>
-      <c r="JH1" s="1">
-        <v>46249</v>
-      </c>
-      <c r="JI1" s="1">
-        <v>46250</v>
-      </c>
-      <c r="JJ1" s="1">
-        <v>46251</v>
-      </c>
-      <c r="JK1" s="1">
-        <v>46252</v>
-      </c>
-      <c r="JL1" s="1">
-        <v>46253</v>
-      </c>
-      <c r="JM1" s="1">
-        <v>46254</v>
-      </c>
-      <c r="JN1" s="1">
-        <v>46255</v>
-      </c>
-      <c r="JO1" s="1">
-        <v>46256</v>
-      </c>
-      <c r="JP1" s="1">
-        <v>46257</v>
-      </c>
-      <c r="JQ1" s="1">
-        <v>46258</v>
-      </c>
-      <c r="JR1" s="1">
-        <v>46259</v>
-      </c>
-      <c r="JS1" s="1">
-        <v>46260</v>
-      </c>
-      <c r="JT1" s="1">
-        <v>46261</v>
-      </c>
-      <c r="JU1" s="1">
-        <v>46262</v>
-      </c>
-      <c r="JV1" s="1">
-        <v>46263</v>
-      </c>
-      <c r="JW1" s="1">
-        <v>46264</v>
-      </c>
-      <c r="JX1" s="1">
-        <v>46265</v>
-      </c>
-      <c r="JY1" s="1">
-        <v>46266</v>
-      </c>
-      <c r="JZ1" s="1">
-        <v>46267</v>
-      </c>
-      <c r="KA1" s="1">
-        <v>46268</v>
-      </c>
-      <c r="KB1" s="1">
-        <v>46269</v>
-      </c>
-      <c r="KC1" s="1">
-        <v>46270</v>
-      </c>
-      <c r="KD1" s="1">
-        <v>46271</v>
-      </c>
-      <c r="KE1" s="1">
-        <v>46272</v>
-      </c>
-      <c r="KF1" s="1">
-        <v>46273</v>
-      </c>
-      <c r="KG1" s="1">
-        <v>46274</v>
-      </c>
-      <c r="KH1" s="1">
-        <v>46275</v>
-      </c>
-      <c r="KI1" s="1">
-        <v>46276</v>
-      </c>
-      <c r="KJ1" s="1">
-        <v>46277</v>
-      </c>
-      <c r="KK1" s="1">
-        <v>46278</v>
-      </c>
-      <c r="KL1" s="1">
-        <v>46279</v>
-      </c>
-      <c r="KM1" s="1">
-        <v>46280</v>
-      </c>
-      <c r="KN1" s="1">
-        <v>46281</v>
-      </c>
-      <c r="KO1" s="1">
-        <v>46282</v>
-      </c>
-      <c r="KP1" s="1">
-        <v>46283</v>
-      </c>
-      <c r="KQ1" s="1">
-        <v>46284</v>
-      </c>
-      <c r="KR1" s="1">
-        <v>46285</v>
-      </c>
-      <c r="KS1" s="1">
-        <v>46286</v>
-      </c>
-      <c r="KT1" s="1">
-        <v>46287</v>
-      </c>
-      <c r="KU1" s="1">
-        <v>46288</v>
-      </c>
-      <c r="KV1" s="1">
-        <v>46289</v>
-      </c>
-      <c r="KW1" s="1">
-        <v>46290</v>
-      </c>
-      <c r="KX1" s="1">
-        <v>46291</v>
-      </c>
-      <c r="KY1" s="1">
-        <v>46292</v>
-      </c>
-      <c r="KZ1" s="1">
-        <v>46293</v>
-      </c>
-      <c r="LA1" s="1">
-        <v>46294</v>
-      </c>
-      <c r="LB1" s="1">
-        <v>46295</v>
-      </c>
-      <c r="LC1" s="1">
-        <v>46296</v>
-      </c>
-      <c r="LD1" s="1">
-        <v>46297</v>
-      </c>
-      <c r="LE1" s="1">
-        <v>46298</v>
-      </c>
-      <c r="LF1" s="1">
-        <v>46299</v>
-      </c>
-      <c r="LG1" s="1">
-        <v>46300</v>
-      </c>
-      <c r="LH1" s="1">
-        <v>46301</v>
-      </c>
-      <c r="LI1" s="1">
-        <v>46302</v>
-      </c>
-      <c r="LJ1" s="1">
-        <v>46303</v>
-      </c>
-      <c r="LK1" s="1">
-        <v>46304</v>
-      </c>
-      <c r="LL1" s="1">
-        <v>46305</v>
-      </c>
-      <c r="LM1" s="1">
-        <v>46306</v>
-      </c>
-      <c r="LN1" s="1">
-        <v>46307</v>
-      </c>
-      <c r="LO1" s="1">
-        <v>46308</v>
-      </c>
-      <c r="LP1" s="1">
-        <v>46309</v>
-      </c>
-      <c r="LQ1" s="1">
-        <v>46310</v>
-      </c>
-      <c r="LR1" s="1">
-        <v>46311</v>
-      </c>
-      <c r="LS1" s="1">
-        <v>46312</v>
-      </c>
-      <c r="LT1" s="1">
-        <v>46313</v>
-      </c>
-      <c r="LU1" s="1">
-        <v>46314</v>
-      </c>
-      <c r="LV1" s="1">
-        <v>46315</v>
-      </c>
-      <c r="LW1" s="1">
-        <v>46316</v>
-      </c>
-      <c r="LX1" s="1">
-        <v>46317</v>
-      </c>
-      <c r="LY1" s="1">
-        <v>46318</v>
-      </c>
-      <c r="LZ1" s="1">
-        <v>46319</v>
-      </c>
-      <c r="MA1" s="1">
-        <v>46320</v>
-      </c>
-      <c r="MB1" s="1">
-        <v>46321</v>
-      </c>
-      <c r="MC1" s="1">
-        <v>46322</v>
-      </c>
-      <c r="MD1" s="1">
-        <v>46323</v>
-      </c>
-      <c r="ME1" s="1">
-        <v>46324</v>
-      </c>
-      <c r="MF1" s="1">
-        <v>46325</v>
-      </c>
-      <c r="MG1" s="1">
         <v>46326</v>
       </c>
     </row>
-    <row r="2" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="DN2">
-        <v>10000</v>
+      <c r="CG2">
+        <v>60000</v>
+      </c>
+      <c r="CI2">
+        <v>1000</v>
+      </c>
+      <c r="CK2">
+        <v>1000</v>
+      </c>
+      <c r="CS2">
+        <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>400000011</v>
       </c>
     </row>
-    <row r="4" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>400000000</v>
       </c>
     </row>
-    <row r="5" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>400000001</v>
       </c>
     </row>
-    <row r="6" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>400000006</v>
       </c>
     </row>
-    <row r="7" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>400000005</v>
       </c>
     </row>
-    <row r="8" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>400000004</v>
       </c>
+      <c r="CG8">
+        <v>5000</v>
+      </c>
     </row>
-    <row r="9" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>400000002</v>
       </c>
     </row>
-    <row r="10" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>400000007</v>
       </c>
+      <c r="CD10">
+        <v>500</v>
+      </c>
     </row>
-    <row r="11" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>400000008</v>
       </c>
     </row>
-    <row r="12" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:257" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>400000009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:257" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>400000990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync project files from local workspace (exclude temp artifacts)
</commit_message>
<xml_diff>
--- a/plan of sales.xlsx
+++ b/plan of sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\so planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159DA231-B524-49A9-BDF2-300B9A385174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8357BE7-E5EF-4EB6-820B-9013B29033A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IW13"/>
+  <dimension ref="A1:IW14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CF1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="CS11" sqref="CS11"/>
+    <sheetView tabSelected="1" topLeftCell="CC1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="CQ13" sqref="CQ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,6 +1215,122 @@
         <v>400000990</v>
       </c>
     </row>
+    <row r="14" spans="1:257" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>400000042</v>
+      </c>
+      <c r="BG14">
+        <v>1000</v>
+      </c>
+      <c r="BH14">
+        <v>1000</v>
+      </c>
+      <c r="BI14">
+        <v>1000</v>
+      </c>
+      <c r="BJ14">
+        <v>1000</v>
+      </c>
+      <c r="BK14">
+        <v>1000</v>
+      </c>
+      <c r="BL14">
+        <v>1000</v>
+      </c>
+      <c r="BM14">
+        <v>1000</v>
+      </c>
+      <c r="BN14">
+        <v>1000</v>
+      </c>
+      <c r="BO14">
+        <v>1000</v>
+      </c>
+      <c r="BP14">
+        <v>1000</v>
+      </c>
+      <c r="BQ14">
+        <v>1000</v>
+      </c>
+      <c r="BR14">
+        <v>1000</v>
+      </c>
+      <c r="BS14">
+        <v>1000</v>
+      </c>
+      <c r="BT14">
+        <v>1000</v>
+      </c>
+      <c r="BU14">
+        <v>1000</v>
+      </c>
+      <c r="BV14">
+        <v>1000</v>
+      </c>
+      <c r="BW14">
+        <v>1000</v>
+      </c>
+      <c r="BX14">
+        <v>1000</v>
+      </c>
+      <c r="BY14">
+        <v>1000</v>
+      </c>
+      <c r="BZ14">
+        <v>1000</v>
+      </c>
+      <c r="CA14">
+        <v>1000</v>
+      </c>
+      <c r="CB14">
+        <v>1000</v>
+      </c>
+      <c r="CC14">
+        <v>1000</v>
+      </c>
+      <c r="CD14">
+        <v>1000</v>
+      </c>
+      <c r="CE14">
+        <v>1000</v>
+      </c>
+      <c r="CF14">
+        <v>1000</v>
+      </c>
+      <c r="CG14">
+        <v>1000</v>
+      </c>
+      <c r="CH14">
+        <v>1000</v>
+      </c>
+      <c r="CI14">
+        <v>1000</v>
+      </c>
+      <c r="CJ14">
+        <v>1000</v>
+      </c>
+      <c r="CK14">
+        <v>1000</v>
+      </c>
+      <c r="CL14">
+        <v>1000</v>
+      </c>
+      <c r="CM14">
+        <v>1000</v>
+      </c>
+      <c r="CN14">
+        <v>1000</v>
+      </c>
+      <c r="CO14">
+        <v>1000</v>
+      </c>
+      <c r="CP14">
+        <v>1000</v>
+      </c>
+      <c r="CQ14">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>